<commit_message>
updated with latest sheet and better connotation prompt
</commit_message>
<xml_diff>
--- a/annotated_connotations.xlsx
+++ b/annotated_connotations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,31 +471,90 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Annotator ID</t>
+          <t>Annotator ID_1</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Bias</t>
+          <t>Bias_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Propaganda</t>
+          <t>Propaganda_1</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Annotator ID_2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Bias_2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Propaganda_2</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Annotator ID_3</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Bias_3</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Propaganda_3</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Annotator ID_4</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Bias_4</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Propaganda_4</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>N-way count bias</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>N-way count propaganda</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Agreement Bias</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Agreement Propaganda</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
           <t>Comments</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>GPT proposal</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>GPT connotation</t>
         </is>
@@ -503,20 +562,20 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2149</v>
+        <v>1706</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B03</t>
+          <t>B02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Arabic</t>
+          <t>Hindi</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>14521</v>
+        <v>1088</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -525,51 +584,70 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>"فتح": تصريحات المدعو حماد تعبر عن انحطاط وطني وأخلاقي وتطالب "حماس" بالاعتذار قالت حركة التحرير الوطني الفلسطيني "فتح"، إن تصريحات المدعو فتحي حماد عضو المكتب السياسي لحماس، تعبر عن مستوى الانحطاط الوطني والأخلاقي، وتأتي في أكثر الظروف الدموية، التي يعيشها شعبنا في الأراضي الفلسطينية كافة، بهدف اشعال الفتنة والحرب الأهلية، وحرف البوصلة الوطنية التي تتمثل في الدفاع عن شعبنا وحقوقنا المشروعة، وأهمية وقف العدوان الغاشم على شعبنا. وأضافت "فتح" في بيان صدر عنها اليوم الأربعاء، "إننا في فتح تحملنا خلال سنوات طويلة هجمات من أمثال المدعو حماد حفاظا على الوحدة الوطنية". وتابعت: يطل بعض قيادات حماس بتصريحات متساوقة مع تصريحات وأهداف نتنياهو الذي يهاجم الرئيس عباس ليلا ونهارا. وأكدت "فتح" أن حركة "حماس" مطالبة الآن بتقديم اعتذار علني للرئيس محمود عباس ومؤسسات الشرعية الفلسطينية والشعب الفلسطيني والدول والشعوب العربية كافة، التي تهتف باسم فلسطين والمقدسات . لمتابعة أخبار فلسطين العاجلة عبر منصة تيلجرام: https://t.me/AwdehTV</t>
+          <t>इजरायल पर नए हमले के लिए हमास फिर तैयार #IsraelHamasConflict | #WarZone</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>"Fatah": The statements of the so-called Hammad express national and moral decadence and demands that "Hamas" apologize. The Palestinian National Liberation Movement "Fatah" said that the statements of the so-called Fathi Hammad, a member of the political bureau of Hamas, express the level of national and moral decadence, and come in the bloodiest circumstances, which Our people are experiencing it in all the Palestinian territories, with the aim of igniting strife and civil war, and distorting the national compass, which is to defend our people and our legitimate rights, and the importance of stopping the brutal aggression against our people. Fatah added in a statement issued on Wednesday, "For many years, we in Fatah have endured attacks from people like Hammad in order to preserve national unity." She continued: Some Hamas leaders make statements consistent with the statements and goals of Netanyahu, who attacks President Abbas day and night. Fatah confirmed that the Hamas movement is now required to make a public apology to President Mahmoud Abbas, the institutions of Palestinian legitimacy, the Palestinian people, and all Arab countries and peoples, which chant in the name of Palestine and the holy sites. To follow breaking Palestinian news via the Telegram platform: https://t.me/AwdehTV</t>
+          <t>Hamas again ready for new attack on Israel #IsraelHamasConflict #WarZone</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>"فتح": تصريحات المدعو حماد تعبر عن انحطاط وطني وأخلاقي وتطالب "حماس" بالاعتذار قالت حركة التحرير الوطني الفلسطيني "فتح"، إن تصريحات المدعو فتحي حماد عضو المكتب السياسي لحماس، تعبر عن مستوى الانحطاط الوطني والأخلاقي، وتأتي في أكثر الظروف الدموية، التي يعيشها شعبنا في الأراضي الفلسطينية كافة، بهدف اشعال الفتنة والحرب الأهلية، وحرف البوصلة الوطنية التي تتمثل في الدفاع عن شعبنا وحقوقنا المشروعة، وأهمية وقف العدوان الغاشم على شعبنا. وأضافت "فتح" في بيان صدر عنها اليوم الأربعاء، "إننا في فتح تحملنا خلال سنوات طويلة هجمات من أمثال المدعو حماد حفاظا على الوحدة الوطنية". وتابعت: يطل بعض قيادات حماس بتصريحات متساوقة مع تصريحات وأهداف نتنياهو الذي يهاجم الرئيس عباس ليلا ونهارا. وأكدت "فتح" أن حركة "حماس" مطالبة الآن بتقديم اعتذار علني للرئيس محمود عباس ومؤسسات الشرعية الفلسطينية والشعب الفلسطيني والدول والشعوب العربية كافة، التي تهتف باسم فلسطين والمقدسات . لمتابعة أخبار فلسطين العاجلة عبر منصة تيلجرام: https://t.me/AwdehTV</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+          <t>حماس مستعدة مرة أخرى لهجوم جديد على إسرائيل # IsraelHamasConflict #منطقة الحرب</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>2</v>
+      </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Biased against Palestine</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>"Fatah": The statements of the so-called[factuality] Hammad express national and moral decadence[negative] and demands that "Hamas" apologize. The Palestinian National Liberation Movement "Fatah" said that the statements of the so-called[factuality] Fathi Hammad, a member of the political bureau of Hamas, express the level of national and moral decadence[negative], and come in the bloodiest[negative] circumstances, which Our people are experiencing it in all the Palestinian territories, with the aim of igniting strife[negative] and civil war[negative], and distorting[negative] the national compass, which is to defend our people and our legitimate rights, and the importance of stopping the brutal[negative] aggression[negative] against our people. Fatah added in a statement issued on Wednesday, "For many years, we in Fatah have endured attacks[negative] from people like Hammad in order to preserve national unity." She continued: Some Hamas leaders make statements consistent with the statements and goals of Netanyahu, who attacks[negative] President Abbas day and night. Fatah confirmed that the Hamas movement is now required to make a public apology to President Mahmoud Abbas, the institutions of Palestinian legitimacy, the Palestinian people, and all Arab countries and peoples, which chant in the name of Palestine and the holy sites. To follow breaking Palestinian news via the Telegram platform: https://t.me/AwdehTV</t>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="n">
+        <v>3</v>
+      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="n">
+        <v>4</v>
+      </c>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Hamas[negative] again ready for new attack on Israel #IsraelHamasConflict #WarZone</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1833</v>
+        <v>1332</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>B03</t>
+          <t>B02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>French</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>673</v>
+        <v>961</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -578,42 +656,61 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>HAPPENING NOW: Pres. Biden delivers remarks after rockets were fired from Gaza into Israel by Hamas militants. https://trib.al/6I7CdnB:=:https://abcnews.go.com/International/live-updates/israel-gaza-hamas/?id=103804516</t>
+          <t>"Je ne mange presque pas"</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>HAPPENING NOW: Pres. Biden delivers remarks after rockets were fired from Gaza into Israel by Hamas militants. https://trib.al/6I7CdnB:=:https://abcnews.go.com/International/live-updates/israel-gaza-hamas/?id=103804516</t>
+          <t>“I hardly eat”</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>يحدث الآن: الرئيس. بايدن يدلي بتصريحاته بعد إطلاق صواريخ من غزة على إسرائيل من قبل نشطاء حماس. https://trib.al/6I7CdnB:=:https://abcnews.go.com/International/live-updates/israel-gaza-hamas/?id=103804516</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>”أنا بالكاد آكل“</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>2</v>
+      </c>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Unbiased</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>HAPPENING NOW: Pres. Biden delivers remarks after rockets were fired[negative] from Gaza into Israel by Hamas militants[negative]. https://trib.al/6I7CdnB:=:https://abcnews.go.com/International/live-updates/israel-gaza-hamas/?id=103804516</t>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
+        <v>4</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>“I hardly eat[negative]”</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>309</v>
+        <v>1144</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B01</t>
+          <t>B02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -622,7 +719,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3530</v>
+        <v>928</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -631,51 +728,70 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>بدأ عملها بخطف جلعاد شاليط، وكانت المسؤولة عن تأمين المحتجزين في صفقة التبادل الأخيرة بين #حماس و #إسرائيل.. فماذا تعرف عن وحدة الظل، أكثر وحدات #القسام سرية؟</t>
+          <t>وصفته "حماس" بـ"الشجاع".. برشلونة تقطع علاقاتها مع إسرائيل حتى الوقف الدائم لإطلاق النار في غزة #الشرق #الشرق_للأخبار</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Her work began with the kidnapping of Gilad Shalit, and she was responsible for securing the detainees in the recent exchange deal between #Hamas and #Israel. What do you know about the Shadow Unit, the most secretive of the #Al-Qassam units?</t>
+          <t>Hamas described him as “brave”... Barcelona cuts ties with Israel until a permanent ceasefire in Gaza #Al-Sharq #Al-Sharq_News</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>بدأ عملها بخطف جلعاد شاليط، وكانت المسؤولة عن تأمين المحتجزين في صفقة التبادل الأخيرة بين #حماس و #إسرائيل.. فماذا تعرف عن وحدة الظل، أكثر وحدات #القسام سرية؟</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+          <t>وصفته "حماس" بـ"الشجاع".. برشلونة تقطع علاقاتها مع إسرائيل حتى الوقف الدائم لإطلاق النار في غزة #الشرق #الشرق_للأخبار</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Unbiased</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Her work began with the kidnapping[negative] of Gilad Shalit, and she was responsible for securing the detainees in the recent exchange deal between #Hamas and #Israel. What do you know about the Shadow Unit, the most secretive[factuality] of the #Al-Qassam units?</t>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>3</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Hamas described him as “brave”[positive]... Barcelona cuts ties with Israel until a permanent ceasefire in Gaza #Al-Sharq[positive] #Al-Sharq_News[positive]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>11796</v>
+        <v>1199</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B14</t>
+          <t>B02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Arabic</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3727</v>
+        <v>4627</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -684,42 +800,61 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The Republican presidential candidates all called for the U.S. to back Israel after the Hamas attack, but they differ in their long-term policies — including their support, or lack thereof, for a two-state solution. Here's what they said: https://nyti.ms/46Zo1gJ:=:https://www.nytimes.com/interactive/2023/10/18/us/politics/republican-candidates-2024-israel.html</t>
+          <t>🗣️قال رئيس الوزراء الإسرائيلي #بنيامين_نتانياهو السبت إن #حركة_حماس "ستدفع ثمنا غير مسبوق" بعد شنها عملية واسعة بالصواريخ والتسلل داخل #إسرائيل. وقال #نتانياهو في بيان: "شنت حماس هذا الصباح هجوما إجراميا مباغتا ضد دولة إسرائيل ومواطنيها". 📲 تابعوا مباشرة على فرانس24 آخر التطورات على مدار الساعة ⬅️https://go.france24.com/IMS:=:https://www.france24.com/ar/%D8%A7%D9%84%D8%B4%D8%B1%D9%82-%D8%A7%D9%84%D8%A3%D9%88%D8%B3%D8%B7/20231007-%D9%82%D8%B7%D8%A7%D8%B9-%D8%BA%D8%B2%D8%A9-%D9%81%D9%84%D8%B3%D8%B7%D9%8A%D9%86-%D8%A5%D8%B3%D8%B1%D8%A7%D8%A6%D9%8A%D9%84-%D9%87%D8%AC%D9%88%D9%85-%D8%B5%D9%88%D8%A7%D8%B1%D9%8A%D8%AE-%D8%AD%D9%85%D8%A7%D8%B3-%D9%86%D8%AA%D8%A7%D9%86%D9%8A%D8%A7%D9%87%D9%88-%D8%B9%D8%B3%D9%82%D9%84%D8%A7%D9%86-%D8%AA%D9%84-%D8%A3%D8%A8%D9%8A%D8%A8</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>The Republican presidential candidates all called for the U.S. to back Israel after the Hamas attack, but they differ in their long-term policies — including their support, or lack thereof, for a two-state solution. Here's what they said: https://nyti.ms/46Zo1gJ:=:https://www.nytimes.com/interactive/2023/10/18/us/politics/republican-candidates-2024-israel.html</t>
+          <t>🗣️Israeli Prime Minister #Benjamin_Netanyahu said on Saturday that #Hamas “will pay an unprecedented price” after launching a massive operation with missiles and infiltration into #Israel. #Netanyahu said in a statement: “This morning, Hamas launched a sudden, criminal attack against the State of Israel and its citizens.” 📲 Follow live on France 24 the latest developments around the clock ⬅️https://go.france24.com/IMS:=:https://www.france24.com/ar/%D8%A7%D9%84%D8%B4% D8%B1%D9%82-%D8%A7%D9%84%D8%A3%D9%88%D8%B3%D8%B7/20231007-%D9%82%D8%B7%D8%A7%D8% B9-%D8%BA%D8%B2%D8%A9-%D9%81%D9%84%D8%B3%D8%B7%D9%8A%D9%86-%D8%A5%D8%B3%D8 %B1%D8%A7%D8%A6%D9%8A%D9%84-%D9%87%D8%AC%D9%88%D9%85-%D8%B5%D9%88%D8%A7%D8 %B1%D9%8A%D8%AE-%D8%AD%D9%85%D8%A7%D8%B3-%D9%86%D8%AA%D8%A7%D9%86%D9%8A%D8 %A7%D9%87%D9%88-%D8%B9%D8%B3%D9%82%D9%84%D8%A7%D9%86-%D8%AA%D9%84-%D8%A3% D8%A8%D9%8A%D8%A8</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>وقد دعا جميع المرشحين الرئاسيين الجمهوريين الولايات المتحدة إلى دعم إسرائيل بعد الهجوم الذي شنته حماس، ولكنهم يختلفون في سياساتهم الطويلة الأمد ــ بما في ذلك دعمهم أو عدم دعمهم لحل الدولتين. إليكم ما قالوه: https://nyti.ms/46Zo1gJ:=:https://www.nytimes.com/interactive/2023/10/18/us/politics/republican-candidates-2024-israel.html</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+          <t>🗣️قال رئيس الوزراء الإسرائيلي #بنيامين_نتانياهو السبت إن #حركة_حماس "ستدفع ثمنا غير مسبوق" بعد شنها عملية واسعة بالصواريخ والتسلل داخل #إسرائيل. وقال #نتانياهو في بيان: "شنت حماس هذا الصباح هجوما إجراميا مباغتا ضد دولة إسرائيل ومواطنيها". 📲 تابعوا مباشرة على فرانس24 آخر التطورات على مدار الساعة ⬅️https://go.france24.com/IMS:=:https://www.france24.com/ar/%D8%A7%D9%84%D8%B4%D8%B1%D9%82-%D8%A7%D9%84%D8%A3%D9%88%D8%B3%D8%B7/20231007-%D9%82%D8%B7%D8%A7%D8%B9-%D8%BA%D8%B2%D8%A9-%D9%81%D9%84%D8%B3%D8%B7%D9%8A%D9%86-%D8%A5%D8%B3%D8%B1%D8%A7%D8%A6%D9%8A%D9%84-%D9%87%D8%AC%D9%88%D9%85-%D8%B5%D9%88%D8%A7%D8%B1%D9%8A%D8%AE-%D8%AD%D9%85%D8%A7%D8%B3-%D9%86%D8%AA%D8%A7%D9%86%D9%8A%D8%A7%D9%87%D9%88-%D8%B9%D8%B3%D9%82%D9%84%D8%A7%D9%86-%D8%AA%D9%84-%D8%A3%D8%A8%D9%8A%D8%A8</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Unbiased</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>The Republican presidential candidates all called for the U.S. to back [positive] Israel after the Hamas attack [negative], but they differ [factuality] in their long-term policies [factuality] — including their support, or lack thereof [negative], for a two-state solution. Here's what they said: https://nyti.ms/46Zo1gJ:=:https://www.nytimes.com/interactive/2023/10/18/us/politics/republican-candidates-2024-israel.html</t>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>🗣️Israeli Prime Minister #Benjamin_Netanyahu said on Saturday that #Hamas “will pay an unprecedented price” after launching a massive operation with missiles and infiltration into #Israel. #Netanyahu said in a statement: “This morning, Hamas launched a sudden, criminal attack against the State of Israel and its citizens.” 📲 Follow live on France 24 the latest developments around the clock ⬅️https://go.france24.com/IMS:=:https://www.france24.com/ar/%D8%A7%D9%84%D8%B4%D8%B1%D9%82-%D8%A7%D9%84%D8%A3%D9%88%D8%B3%D8%B7/20231007-%D9%82%D8%B7%D8%A7%D8%B9-%D8%BA%D8%B2%D8%A9-%D9%81%D9%84%D8%B3%D8%B7%D9%8A%D9%86-%D8%A5%D8%B3%D8%B1%D8%A7%D8%A6%D9%8A%D9%84-%D9%87%D8%AC%D9%88%D9%85-%D8%B5%D9%88%D8%A7%D8%B1%D9%8A%D8%AE-%D8%AD%D9%85%D8%A7%D8%B3-%D9%86%D8%AA%D8%A7%D9%86%D9%8A%D8%A7%D9%87%D9%88-%D8%B9%D8%B3%D9%82%D9%84%D8%A7%D9%86-%D8%AA%D9%84-%D8%A3%D8%A8%D9%8A%D8%A8</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>12011</v>
+        <v>297</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B14</t>
+          <t>B01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -728,7 +863,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9325</v>
+        <v>2381</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -737,32 +872,51 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>منذ 15 عاماً.. 4 حروب اندلعت بين الفلسطينيين والإسرائيليين</t>
+          <t>🔴 أعلن مصدر طبي إسرائيلي السبت سقوط 70 قتيلا على الأقل في إسرائيل في عمليات التوغل التي نفذتها #حركة_حماس، فيما قتل 198 فلسطينيا على الأقل في #غزة بغارات جوية على القطاع.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>15 years ago... 4 wars broke out between Palestinians and Israelis</t>
+          <t>🔴 An Israeli medical source announced on Saturday that at least 70 people were killed in Israel in the incursions carried out by #Hamas, while at least 198 Palestinians were killed in #Gaza in air strikes on the Strip.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>منذ 15 عاماً.. 4 حروب اندلعت بين الفلسطينيين والإسرائيليين</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>🔴 أعلن مصدر طبي إسرائيلي السبت سقوط 70 قتيلا على الأقل في إسرائيل في عمليات التوغل التي نفذتها #حركة_حماس، فيما قتل 198 فلسطينيا على الأقل في #غزة بغارات جوية على القطاع.</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Unbiased</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>15 years ago... 4 wars[negative] broke out[negative] between Palestinians and Israelis</t>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
+        <v>4</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>An Israeli medical source announced on Saturday that at least 70 people were killed in Israel in the incursions carried out by #Hamas, while at least 198 Palestinians were killed in #Gaza in air strikes on the Strip.</t>
         </is>
       </c>
     </row>

</xml_diff>